<commit_message>
Magnirrostris and conirrostris distributions
</commit_message>
<xml_diff>
--- a/Data/Raw/Magni Distribution.xlsx
+++ b/Data/Raw/Magni Distribution.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\R\Tribulus\Tribulus mericarp morphology\Tribulus-mericarp-morphology\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4649233-E1CE-42D6-89CE-6FF860308003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727371C4-98AF-4A23-8D62-10E19BC3625F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-120" windowWidth="23256" windowHeight="12576" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Islands with Magnis</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Baltra</t>
   </si>
@@ -81,9 +78,6 @@
     <t>Seymour Norte</t>
   </si>
   <si>
-    <t>Islands without Magnis</t>
-  </si>
-  <si>
     <t>Floreana</t>
   </si>
   <si>
@@ -100,6 +94,18 @@
   </si>
   <si>
     <t>Enderby</t>
+  </si>
+  <si>
+    <t>Islands without Magnis and Coriorrostris</t>
+  </si>
+  <si>
+    <t>Gardner</t>
+  </si>
+  <si>
+    <t>Daphne Major &lt;1983</t>
+  </si>
+  <si>
+    <t>Islands with Magnis and Cornirrostris</t>
   </si>
 </sst>
 </file>
@@ -451,77 +457,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8B28B9-2EFA-4490-BD21-0ABE0D1E7E4C}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -529,32 +535,40 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Lv flw mer"
</commit_message>
<xml_diff>
--- a/Data/Raw/Magni Distribution.xlsx
+++ b/Data/Raw/Magni Distribution.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\R\Tribulus\Tribulus mericarp morphology\Tribulus-mericarp-morphology\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727371C4-98AF-4A23-8D62-10E19BC3625F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4649233-E1CE-42D6-89CE-6FF860308003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
+    <workbookView xWindow="-23148" yWindow="-120" windowWidth="23256" windowHeight="12576" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Islands with Magnis</t>
+  </si>
   <si>
     <t>Baltra</t>
   </si>
@@ -78,6 +81,9 @@
     <t>Seymour Norte</t>
   </si>
   <si>
+    <t>Islands without Magnis</t>
+  </si>
+  <si>
     <t>Floreana</t>
   </si>
   <si>
@@ -94,18 +100,6 @@
   </si>
   <si>
     <t>Enderby</t>
-  </si>
-  <si>
-    <t>Islands without Magnis and Coriorrostris</t>
-  </si>
-  <si>
-    <t>Gardner</t>
-  </si>
-  <si>
-    <t>Daphne Major &lt;1983</t>
-  </si>
-  <si>
-    <t>Islands with Magnis and Cornirrostris</t>
   </si>
 </sst>
 </file>
@@ -457,77 +451,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8B28B9-2EFA-4490-BD21-0ABE0D1E7E4C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A3" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -535,40 +529,32 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Distribution of magni and cornirrostris finches in galapagos
</commit_message>
<xml_diff>
--- a/Data/Raw/Magni Distribution.xlsx
+++ b/Data/Raw/Magni Distribution.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\R\Tribulus\Tribulus mericarp morphology\Tribulus-mericarp-morphology\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4649233-E1CE-42D6-89CE-6FF860308003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727371C4-98AF-4A23-8D62-10E19BC3625F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-120" windowWidth="23256" windowHeight="12576" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Islands with Magnis</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Baltra</t>
   </si>
@@ -81,9 +78,6 @@
     <t>Seymour Norte</t>
   </si>
   <si>
-    <t>Islands without Magnis</t>
-  </si>
-  <si>
     <t>Floreana</t>
   </si>
   <si>
@@ -100,6 +94,18 @@
   </si>
   <si>
     <t>Enderby</t>
+  </si>
+  <si>
+    <t>Islands without Magnis and Coriorrostris</t>
+  </si>
+  <si>
+    <t>Gardner</t>
+  </si>
+  <si>
+    <t>Daphne Major &lt;1983</t>
+  </si>
+  <si>
+    <t>Islands with Magnis and Cornirrostris</t>
   </si>
 </sst>
 </file>
@@ -451,77 +457,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8B28B9-2EFA-4490-BD21-0ABE0D1E7E4C}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -529,32 +535,40 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the finch distribution file to create a table in the markdown
</commit_message>
<xml_diff>
--- a/Data/Raw/Magni Distribution.xlsx
+++ b/Data/Raw/Magni Distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\R\Tribulus\Tribulus mericarp morphology\Tribulus-mericarp-morphology\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727371C4-98AF-4A23-8D62-10E19BC3625F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5047B7B4-97E8-4FE5-AA4B-8D346E0F89CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
+    <workbookView xWindow="-21828" yWindow="2412" windowWidth="21600" windowHeight="11208" xr2:uid="{9677C0A9-D303-4E6C-8990-322C0FF61604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8B28B9-2EFA-4490-BD21-0ABE0D1E7E4C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,103 +477,103 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B15">
-    <sortCondition ref="A3:A15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
+    <sortCondition ref="A2:A14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>